<commit_message>
adding and incorporating similarity and embedding changes
</commit_message>
<xml_diff>
--- a/Heuristic2/bgelarge_cross_encode/final_rank_30.xlsx
+++ b/Heuristic2/bgelarge_cross_encode/final_rank_30.xlsx
@@ -28,85 +28,85 @@
     <t>Bill &amp; Melinda Gates Foundation</t>
   </si>
   <si>
+    <t>Y Combinator</t>
+  </si>
+  <si>
+    <t>Reach Capital</t>
+  </si>
+  <si>
+    <t>Google for Education</t>
+  </si>
+  <si>
     <t>U.S. Dept. of Education (EIR Program)</t>
   </si>
   <si>
-    <t>Reach Capital</t>
+    <t>National Science Foundation (NSF)</t>
   </si>
   <si>
     <t>500 Global Flagship VC (non-accelerator checks)</t>
   </si>
   <si>
+    <t>IES SBIR (ED/IES)</t>
+  </si>
+  <si>
+    <t>500 Global (seed/accelerator)</t>
+  </si>
+  <si>
+    <t>Buffalo Sabres Foundation</t>
+  </si>
+  <si>
+    <t>TGR Foundation (Tiger Woods)</t>
+  </si>
+  <si>
+    <t>Berkeley SkyDeck Fund (UC Berkeley)</t>
+  </si>
+  <si>
+    <t>Penn State University - Outreach &amp; Engagement</t>
+  </si>
+  <si>
     <t>Chan Zuckerberg Initiative (CZI)</t>
   </si>
   <si>
-    <t>Google for Education</t>
-  </si>
-  <si>
-    <t>National Science Foundation (NSF)</t>
-  </si>
-  <si>
-    <t>IES SBIR (ED/IES)</t>
-  </si>
-  <si>
-    <t>Y Combinator</t>
-  </si>
-  <si>
-    <t>NSF SBIR (“America’s Seed Fund”)</t>
-  </si>
-  <si>
-    <t>500 Global (seed/accelerator)</t>
-  </si>
-  <si>
-    <t>Berkeley SkyDeck Fund (UC Berkeley)</t>
-  </si>
-  <si>
-    <t>New York City FC - City in the Community Foundation</t>
-  </si>
-  <si>
-    <t>University of Wisconsin-Madison - Community Relations</t>
-  </si>
-  <si>
-    <t>MIT Solve (Global Learning &amp; education tracks)</t>
-  </si>
-  <si>
-    <t>LA Clippers Foundation</t>
-  </si>
-  <si>
-    <t>Portland Timbers Community Fund</t>
-  </si>
-  <si>
-    <t>Columbus Blue Jackets Foundation</t>
-  </si>
-  <si>
-    <t>New York Yankees Foundation</t>
-  </si>
-  <si>
-    <t>New York Islanders Children's Foundation</t>
-  </si>
-  <si>
-    <t>New York Jets Foundation</t>
+    <t>Nashville Predators Foundation</t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers Foundation</t>
+  </si>
+  <si>
+    <t>NFL Foundation</t>
+  </si>
+  <si>
+    <t>San Jose Sharks Foundation</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs - Spurs Give</t>
+  </si>
+  <si>
+    <t>Indiana Pacers Foundation</t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers Community Foundation</t>
+  </si>
+  <si>
+    <t>Austin FC - 4ATX Foundation</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens Foundation</t>
+  </si>
+  <si>
+    <t>Toronto FC - MLSE Foundation</t>
   </si>
   <si>
     <t>Houston Texans Foundation</t>
   </si>
   <si>
-    <t>Duke University - Duke-Durham Neighborhood Partnership</t>
-  </si>
-  <si>
-    <t>Seattle Seahawks - Spirit of 12</t>
-  </si>
-  <si>
-    <t>MLB Players Trust</t>
-  </si>
-  <si>
-    <t>Boston Red Sox Foundation</t>
-  </si>
-  <si>
-    <t>DonorsChoose (technology classroom projects)</t>
-  </si>
-  <si>
-    <t>Green Bay Packers Foundation</t>
+    <t>Philadelphia Eagles Foundation</t>
+  </si>
+  <si>
+    <t>Oakland Roots SC</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars Foundation</t>
   </si>
   <si>
     <t>Florida State University Research Foundation</t>

</xml_diff>